<commit_message>
DA17 | Day 8
</commit_message>
<xml_diff>
--- a/Batch/17/Day_8_Date_functions.xlsx
+++ b/Batch/17/Day_8_Date_functions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Work\Acciojob\Modules\Excel\Batch\15\Curriculum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\OneDrive\Work\Acciojob\Modules\Excel\Batch\17\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C256EE-784A-4781-B7B7-2239F988462A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32208D0B-26C5-442D-8EEA-C6D384B2CC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="30" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>Data Used in Formula</t>
   </si>
@@ -213,6 +213,15 @@
   <si>
     <t>NETWORKDAY uses the start date and end date and returns the total working days. This does not includes weekends (Saturday and Sunday) and the specified holidays (d4:d6)</t>
   </si>
+  <si>
+    <t>No Of Days</t>
+  </si>
+  <si>
+    <t>No Of working days considering Saturday and Sunday as weekend</t>
+  </si>
+  <si>
+    <t>No of Working days considering Monday as weekend</t>
+  </si>
 </sst>
 </file>
 
@@ -222,7 +231,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,34 +239,47 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF002060"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -265,6 +287,7 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -365,94 +388,95 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="18" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="18" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3124,11 +3148,11 @@
   <sheetData>
     <row r="1" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
     </row>
     <row r="3" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="13" t="s">
@@ -5394,7 +5418,7 @@
       </c>
       <c r="C7" s="20">
         <f ca="1">NOW() +B3</f>
-        <v>45679.918603240738</v>
+        <v>45763.895796643519</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>32</v>
@@ -7511,32 +7535,32 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="B1:D1000"/>
+  <dimension ref="B1:E1000"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="8.73046875" customWidth="1"/>
-    <col min="2" max="2" width="21.86328125" customWidth="1"/>
-    <col min="3" max="3" width="14.53125" customWidth="1"/>
-    <col min="4" max="4" width="36" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.9296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.73046875" customWidth="1"/>
     <col min="6" max="6" width="9.1328125" customWidth="1"/>
     <col min="7" max="26" width="8.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
-    <row r="2" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="31" t="s">
+    <row r="1" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B2" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-    </row>
-    <row r="3" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+    </row>
+    <row r="3" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B3" s="5" t="s">
         <v>41</v>
       </c>
@@ -7547,7 +7571,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B4" s="21">
         <v>41699</v>
       </c>
@@ -7558,26 +7582,26 @@
         <v>41701</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="25"/>
       <c r="C5" s="26"/>
       <c r="D5" s="21">
         <v>41719</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="25"/>
       <c r="C6" s="26"/>
       <c r="D6" s="21">
         <v>41772</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="16"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="19" t="s">
         <v>1</v>
       </c>
@@ -7588,51 +7612,65 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="42" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:5" ht="42" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="6"/>
       <c r="C9" s="27"/>
       <c r="D9" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:5" ht="57.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="6"/>
       <c r="C10" s="27"/>
       <c r="D10" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="12" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="9"/>
       <c r="C12" s="10"/>
-      <c r="D12" s="11">
+      <c r="D12" s="11"/>
+    </row>
+    <row r="13" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B13" s="12"/>
+      <c r="C13" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13">
         <f>C4-B4</f>
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="12"/>
-      <c r="D13">
+    <row r="14" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B14" s="12"/>
+      <c r="C14" s="28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14">
         <f>NETWORKDAYS(B4,C4,D4:D6)</f>
         <v>68</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="12"/>
-      <c r="D14">
-        <f>NETWORKDAYS.INTL(B4,C4,2,D4:D6)</f>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="15" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E14">
+        <f>NETWORKDAYS(B4,C4)</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="12"/>
-    </row>
-    <row r="16" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C15" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15">
+        <f>NETWORKDAYS.INTL(B4,C4,12,D4:D6)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="12"/>
     </row>
     <row r="17" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>

</xml_diff>